<commit_message>
fix bug: Multiple cell comments in one cell are not allowed
</commit_message>
<xml_diff>
--- a/src/test/resources/export-goods.xlsx
+++ b/src/test/resources/export-goods.xlsx
@@ -17,6 +17,11 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <t>测试A1单元格备注功能</t>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0">
       <text>
         <t>测试B1单元格备注功能</t>

</xml_diff>

<commit_message>
small change: add 100 rows more for cell constraint
</commit_message>
<xml_diff>
--- a/src/test/resources/export-goods.xlsx
+++ b/src/test/resources/export-goods.xlsx
@@ -42,7 +42,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+  <si>
+    <t>商品名</t>
+  </si>
+  <si>
+    <t>单位</t>
+  </si>
+  <si>
+    <t>规格</t>
+  </si>
+  <si>
+    <t>生产厂家</t>
+  </si>
+  <si>
+    <t>生产时间</t>
+  </si>
+  <si>
+    <t>出厂日期</t>
+  </si>
+  <si>
+    <t>数量</t>
+  </si>
+  <si>
+    <t>价格</t>
+  </si>
+  <si>
+    <t>售价</t>
+  </si>
+  <si>
+    <t>类型</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>青霉素</t>
+  </si>
+  <si>
+    <t>盒</t>
+  </si>
+  <si>
+    <t>3片/盒</t>
+  </si>
+  <si>
+    <t>贵州  百灵</t>
+  </si>
+  <si>
+    <t>西药</t>
+  </si>
+  <si>
+    <t>板蓝根</t>
+  </si>
+  <si>
+    <t>12包/盒</t>
+  </si>
+  <si>
+    <t>广  州白云山</t>
+  </si>
+  <si>
+    <t>中药</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51,13 +112,18 @@
     <numFmt numFmtId="164" formatCode="yyyy-MM-dd HH:mm:ss"/>
     <numFmt numFmtId="165" formatCode="MM/dd/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -142,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment wrapText="false"/>
@@ -171,6 +237,9 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment wrapText="false"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="false"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="false" horizontal="left"/>
       <protection locked="false"/>
@@ -214,6 +283,10 @@
       <protection locked="false"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="false" horizontal="left"/>
+      <protection locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="false" horizontal="right"/>
       <protection locked="false"/>
     </xf>
@@ -244,6 +317,10 @@
       <protection locked="false"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="false" horizontal="left"/>
+      <protection locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="false" horizontal="left"/>
       <protection locked="false"/>
     </xf>
@@ -257,145 +334,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.20703125" customWidth="true"/>
+    <col min="1" max="1" width="8.421875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="6.0" customWidth="true"/>
-    <col min="3" max="3" width="8.1640625" customWidth="true"/>
+    <col min="3" max="3" width="8.1640625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="6.0" customWidth="true"/>
-    <col min="5" max="5" width="21.1328125" customWidth="true"/>
-    <col min="6" max="6" width="12.23828125" customWidth="true"/>
-    <col min="7" max="7" width="6.0859375" customWidth="true"/>
-    <col min="8" max="8" width="7.41796875" customWidth="true" hidden="true"/>
-    <col min="9" max="9" width="6.2578125" customWidth="true"/>
+    <col min="5" max="5" width="21.1328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="12.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="6.0859375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="7.41796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="9" max="9" width="6.2578125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="6.0859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>商品名</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>单位</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>规格</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>生产厂家</t>
-        </is>
-      </c>
-      <c r="E1" s="5" t="inlineStr">
-        <is>
-          <t>生产时间</t>
-        </is>
-      </c>
-      <c r="F1" s="6" t="inlineStr">
-        <is>
-          <t>出厂日期</t>
-        </is>
-      </c>
-      <c r="G1" s="7" t="inlineStr">
-        <is>
-          <t>数量</t>
-        </is>
-      </c>
-      <c r="H1" s="8" t="inlineStr">
-        <is>
-          <t>价格</t>
-        </is>
-      </c>
-      <c r="I1" s="9" t="inlineStr">
-        <is>
-          <t>售价</t>
-        </is>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
-        <is>
-          <t>感冒灵颗粒</t>
-        </is>
-      </c>
-      <c r="B2" s="11" t="inlineStr">
-        <is>
-          <t>盒</t>
-        </is>
-      </c>
-      <c r="C2" s="12" t="inlineStr">
-        <is>
-          <t>3片/盒</t>
-        </is>
-      </c>
-      <c r="D2" s="13" t="inlineStr">
-        <is>
-          <t>贵州  百灵</t>
-        </is>
-      </c>
-      <c r="E2" s="15" t="n">
+      <c r="A2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="n" s="16">
         <v>40139.0</v>
       </c>
-      <c r="F2" s="17" t="n">
+      <c r="F2" t="n" s="18">
         <v>40139.0</v>
       </c>
-      <c r="G2" s="18" t="n">
+      <c r="G2" s="19" t="n">
         <v>0.0</v>
       </c>
-      <c r="H2" s="19" t="n">
+      <c r="H2" s="20" t="n">
         <v>1.0E-4</v>
       </c>
-      <c r="I2" s="20" t="n">
+      <c r="I2" s="21" t="n">
         <v>19.34680938720703</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="21" t="inlineStr">
-        <is>
-          <t>板蓝根</t>
-        </is>
-      </c>
-      <c r="B3" s="22" t="inlineStr">
-        <is>
-          <t>盒</t>
-        </is>
-      </c>
-      <c r="C3" s="23" t="inlineStr">
-        <is>
-          <t>12包/盒</t>
-        </is>
-      </c>
-      <c r="D3" s="24" t="inlineStr">
-        <is>
-          <t>广  州白云山</t>
-        </is>
-      </c>
-      <c r="E3" s="26" t="n">
+      <c r="A3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="n" s="28">
         <v>43617.0</v>
       </c>
-      <c r="F3" s="28" t="n">
+      <c r="F3" t="n" s="30">
         <v>43617.0</v>
       </c>
-      <c r="G3" s="29" t="n">
+      <c r="G3" s="31" t="n">
         <v>135.0</v>
       </c>
-      <c r="H3" s="30" t="n">
+      <c r="H3" s="32" t="n">
         <v>45.56</v>
       </c>
-      <c r="I3" s="31" t="n">
+      <c r="I3" s="33" t="n">
         <v>70.0</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="decimal" operator="between" sqref="I2:I104" allowBlank="true" errorStyle="stop" showErrorMessage="true">
+      <formula1>10</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="J2:J104" allowBlank="true" errorStyle="stop" showErrorMessage="true">
+      <formula1>"西药,中药"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
1. add required in ExcellCell 2. add notice in ExcellSheet
</commit_message>
<xml_diff>
--- a/src/test/resources/export-goods.xlsx
+++ b/src/test/resources/export-goods.xlsx
@@ -17,22 +17,22 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A2" authorId="0">
       <text>
         <t>测试A1单元格备注功能</t>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B2" authorId="0">
       <text>
         <t>测试B1单元格备注功能</t>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D2" authorId="0">
       <text>
         <t>测试单元格宽度、自动换行、备注功能</t>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G2" authorId="0">
       <text>
         <t>测试G1单元格备注功能</t>
       </text>
@@ -42,7 +42,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">填写须知：
+1、不能增加、删除列；
+3、不能修改灰色单元格；
+2、红色字段为必填字段，黑色字段为选填字段；
+</t>
+  </si>
   <si>
     <t>商品名</t>
   </si>
@@ -112,7 +119,7 @@
     <numFmt numFmtId="164" formatCode="yyyy-MM-dd HH:mm:ss"/>
     <numFmt numFmtId="165" formatCode="MM/dd/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -122,18 +129,25 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="14.0"/>
-      <b val="true"/>
+      <sz val="16.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -171,7 +185,7 @@
       <b val="true"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +207,23 @@
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
         <bgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="22"/>
+        <bgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="22"/>
       </patternFill>
     </fill>
   </fills>
@@ -208,10 +239,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment wrapText="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment wrapText="true" horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment wrapText="false"/>
@@ -220,11 +251,11 @@
       <alignment wrapText="false"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment wrapText="false"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment wrapText="false"/>
     </xf>
@@ -240,9 +271,12 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment wrapText="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="false" horizontal="left"/>
-      <protection locked="false"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="false" horizontal="left"/>
+      <protection locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="false" horizontal="right"/>
@@ -282,9 +316,9 @@
       <alignment wrapText="false" horizontal="left"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="false" horizontal="left"/>
-      <protection locked="false"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="false" horizontal="left"/>
+      <protection locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="false" horizontal="right"/>
@@ -334,7 +368,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -352,109 +386,117 @@
     <col min="10" max="10" width="6.0859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="108.5" customHeight="true">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="n" s="16">
-        <v>40139.0</v>
-      </c>
-      <c r="F2" t="n" s="18">
-        <v>40139.0</v>
-      </c>
-      <c r="G2" s="19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H2" s="20" t="n">
-        <v>1.0E-4</v>
-      </c>
-      <c r="I2" s="21" t="n">
-        <v>19.34680938720703</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>15</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="n" s="17">
+        <v>40139.0</v>
+      </c>
+      <c r="F3" t="n" s="19">
+        <v>40139.0</v>
+      </c>
+      <c r="G3" s="20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" s="21" t="n">
+        <v>1.0E-4</v>
+      </c>
+      <c r="I3" s="22" t="n">
+        <v>19.34680938720703</v>
+      </c>
+      <c r="J3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="25" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="B4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="n" s="28">
+      <c r="D4" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="n" s="29">
         <v>43617.0</v>
       </c>
-      <c r="F3" t="n" s="30">
+      <c r="F4" t="n" s="31">
         <v>43617.0</v>
       </c>
-      <c r="G3" s="31" t="n">
+      <c r="G4" s="32" t="n">
         <v>135.0</v>
       </c>
-      <c r="H3" s="32" t="n">
+      <c r="H4" s="33" t="n">
         <v>45.56</v>
       </c>
-      <c r="I3" s="33" t="n">
+      <c r="I4" s="34" t="n">
         <v>70.0</v>
       </c>
-      <c r="J3" s="34" t="s">
-        <v>19</v>
+      <c r="J4" s="35" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="between" sqref="I2:I104" allowBlank="true" errorStyle="stop" showErrorMessage="true">
+    <dataValidation type="decimal" operator="between" sqref="I3:I104" allowBlank="true" errorStyle="stop" showErrorMessage="true">
       <formula1>10</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="J2:J104" allowBlank="true" errorStyle="stop" showErrorMessage="true">
+    <dataValidation type="list" sqref="J3:J104" allowBlank="true" errorStyle="stop" showErrorMessage="true">
       <formula1>"西药,中药"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>